<commit_message>
major refactoring, making code readable
</commit_message>
<xml_diff>
--- a/data/employees.xlsx
+++ b/data/employees.xlsx
@@ -4,17 +4,19 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="17610"/>
+    <workbookView windowWidth="19200" windowHeight="17610" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Contracts" sheetId="2" r:id="rId2"/>
+    <sheet name="Jobs" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="74">
   <si>
     <t>Vārds</t>
   </si>
@@ -23,6 +25,707 @@
   </si>
   <si>
     <t>Jānis</t>
+  </si>
+  <si>
+    <t>Darbs</t>
+  </si>
+  <si>
+    <t>Samaksa</t>
+  </si>
+  <si>
+    <t>Miks</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="186"/>
+      </rPr>
+      <t>FĀZĪTES PULĒŠANA ; T/M</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="186"/>
+      </rPr>
+      <t>PULĒŠANA -TAISNA KANTE ; T/M</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="186"/>
+      </rPr>
+      <t>PULĒŠANA - TAISNA KANTE AR R ; T/M</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="186"/>
+      </rPr>
+      <t>PULĒŠANA - PUSAPĻA KANTE ; T/M</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="186"/>
+      </rPr>
+      <t>PULĒŠANA - PUSAPĻA KANTE AR R ; T/M</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="186"/>
+      </rPr>
+      <t>PULĒŠANA - PILNS APLIS ; T/M</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="186"/>
+      </rPr>
+      <t>PULĒŠANA - PILNS APLIS AR R ; T/M</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="186"/>
+      </rPr>
+      <t>KANTE AR LIELO FĀZI ; T/M</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="186"/>
+      </rPr>
+      <t>KANTE AR NOAPAĻOTĀM FĀZĒM ; T/M</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="186"/>
+      </rPr>
+      <t>PULĒŠANA - PROFILS ; T/M</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="186"/>
+      </rPr>
+      <t>VIRSMAS ANTIĶĒŠANA - MARMORS ; m2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="186"/>
+      </rPr>
+      <t>VIRSMAS ANTIĶĒŠANA - GRANĪTS ; m2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="186"/>
+      </rPr>
+      <t>VIRSMAS IMPREGNĒŠANA ; m2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="186"/>
+      </rPr>
+      <t>VIRSMAS PĀRPULĒŠANA ; m2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="186"/>
+      </rPr>
+      <t>KANELURU IZPULĒŠANA ; T/M</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="186"/>
+      </rPr>
+      <t>LĪMĒŠANA AR FĀZĪTI ; T/M</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="186"/>
+      </rPr>
+      <t>SLĪPĒŠANA 45º ; T/M</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="186"/>
+      </rPr>
+      <t>LĪMĒŠANA BEZ FĀZĪTES ; T/M</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="186"/>
+      </rPr>
+      <t>LĪMĒTAS KANTES PULĒŠANA ; T/M</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="186"/>
+      </rPr>
+      <t>PADZIĻINĀJUMU IEFRĒZĒŠANA ; m2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="186"/>
+      </rPr>
+      <t>IZGRIEZUMU IZZĀĢĒŠANA ; GAB.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="186"/>
+      </rPr>
+      <t>IZGRIEZUMU IZPULĒŠANA ; GAB.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="186"/>
+      </rPr>
+      <t>URBUMS R = 8 -10mm ; GAB.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="186"/>
+      </rPr>
+      <t>URBUMS R = 35mm ; GAB.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="186"/>
+      </rPr>
+      <t>URBUMS R = VIRS 50mm ; GAB.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="186"/>
+      </rPr>
+      <t>ARMATŪRAS IELĪMĒŠANA ; GAB.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="186"/>
+      </rPr>
+      <t>ŠABLONU IZGATAVOŠANA ; GAB.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="186"/>
+      </rPr>
+      <t>GRAUŠANA/SADZĪŠANA ; h</t>
+    </r>
+  </si>
+  <si>
+    <t>Montāža</t>
+  </si>
+  <si>
+    <t>Izgatavošana</t>
+  </si>
+  <si>
+    <t>Uzmērīšana/Šablona noņemšana</t>
+  </si>
+  <si>
+    <t>Darbs cehā</t>
+  </si>
+  <si>
+    <t>Andrejs</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Modris</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="186"/>
+      </rPr>
+      <t>FĀZĪTES PULĒŠANA ; T/M</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="186"/>
+      </rPr>
+      <t>PULĒŠANA -TAISNA KANTE ; T/M</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="186"/>
+      </rPr>
+      <t>PULĒŠANA - TAISNA KANTE AR R ; T/M</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="186"/>
+      </rPr>
+      <t>PULĒŠANA - PUSAPĻA KANTE ; T/M</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="186"/>
+      </rPr>
+      <t>PULĒŠANA - PUSAPĻA KANTE AR R ; T/M</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="186"/>
+      </rPr>
+      <t>PULĒŠANA - PILNS APLIS ; T/M</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="186"/>
+      </rPr>
+      <t>PULĒŠANA - PILNS APLIS AR R ; T/M</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="186"/>
+      </rPr>
+      <t>KANTE AR LIELO FĀZI ; T/M</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="186"/>
+      </rPr>
+      <t>KANTE AR NOAPAĻOTĀM FĀZĒM ; T/M</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="186"/>
+      </rPr>
+      <t>PULĒŠANA - PROFILS ; T/M</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="186"/>
+      </rPr>
+      <t>VIRSMAS ANTIĶĒŠANA - MARMORS ; m2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="186"/>
+      </rPr>
+      <t>VIRSMAS ANTIĶĒŠANA - GRANĪTS ; m2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="186"/>
+      </rPr>
+      <t>VIRSMAS IMPREGNĒŠANA ; m2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="186"/>
+      </rPr>
+      <t>VIRSMAS PĀRPULĒŠANA ; m2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="186"/>
+      </rPr>
+      <t>KANELURU IZPULĒŠANA ; T/M</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="186"/>
+      </rPr>
+      <t>LĪMĒŠANA AR FĀZĪTI ; T/M</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="186"/>
+      </rPr>
+      <t>SLĪPĒŠANA 45º ; T/M</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="186"/>
+      </rPr>
+      <t>LĪMĒŠANA BEZ FĀZĪTES ; T/M</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="186"/>
+      </rPr>
+      <t>LĪMĒTAS KANTES PULĒŠANA ; T/M</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="186"/>
+      </rPr>
+      <t>PADZIĻINĀJUMU IEFRĒZĒŠANA ; m2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="186"/>
+      </rPr>
+      <t>IZGRIEZUMU IZZĀĢĒŠANA ; GAB.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="186"/>
+      </rPr>
+      <t>IZGRIEZUMU IZPULĒŠANA ; GAB.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="186"/>
+      </rPr>
+      <t>URBUMS R = 8 -10mm ; GAB.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="186"/>
+      </rPr>
+      <t>URBUMS R = 35mm ; GAB.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="186"/>
+      </rPr>
+      <t>URBUMS R = VIRS 50mm ; GAB.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="186"/>
+      </rPr>
+      <t>ARMATŪRAS IELĪMĒŠANA ; GAB.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="186"/>
+      </rPr>
+      <t>ŠABLONU IZGATAVOŠANA ; GAB.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="186"/>
+      </rPr>
+      <t>GRAUŠANA/SADZĪŠANA ; h</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Montāža</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Izgatavošana</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Uzmērīšana/Šablona noņemšana</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Darbs cehā</t>
+    </r>
+  </si>
+  <si>
+    <t>Darbu saraksts</t>
+  </si>
+  <si>
+    <t>Prioritāte anketā</t>
   </si>
 </sst>
 </file>
@@ -35,7 +738,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -45,10 +748,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -194,6 +896,18 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <charset val="186"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <charset val="186"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -498,19 +1212,19 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -519,7 +1233,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -643,8 +1357,10 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -993,8 +1709,8 @@
   <sheetPr/>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="2"/>
@@ -1018,4 +1734,1384 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C97"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="6.57142857142857" style="1" customWidth="1"/>
+    <col min="2" max="2" width="45.5714285714286" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.14285714285714" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.14285714285714" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C40" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C41" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C43" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C44" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C45" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C46" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C47" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C48" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C49" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C50" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C51" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C52" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C53" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C54" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C55" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C56" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C57" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C58" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C59" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C60" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C61" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C62" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C63" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C64" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C65" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C66" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C67" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C68" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C69" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C70" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C71" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C72" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C73" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C74" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C75" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C76" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C77" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C78" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C79" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C80" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C81" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C82" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C83" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C84" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C85" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C86" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C87" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C88" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C89" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C90" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C91" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C92" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C93" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C94" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C95" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C96" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C97" s="2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>Jobs!$A:$A</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="41.8571428571429" customWidth="1"/>
+    <col min="2" max="2" width="17.2857142857143" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>